<commit_message>
arrange the data correctlly
</commit_message>
<xml_diff>
--- a/.idea/fedInvestments.xlsx
+++ b/.idea/fedInvestments.xlsx
@@ -1,37 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadar\IdeaProjects\.idea\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FE0029-FEED-4F5A-B718-02D4197051FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fed_investments</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,94 +71,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,186 +396,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>fed_investments</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>20070900</v>
-      </c>
-      <c r="B2" t="n">
-        <v>12801000000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>20071000</v>
-      </c>
-      <c r="B3" t="n">
-        <v>12801000000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>20071100</v>
-      </c>
-      <c r="B4" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>20071200</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>20071300</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>20071400</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1732000000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>20071500</v>
-      </c>
-      <c r="B8" t="n">
-        <v>6001000000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>20071600</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1201000000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>20071700</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1732000000</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>20071800</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>20071900</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>20072000</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>20072100</v>
-      </c>
-      <c r="B14" t="n">
-        <v>12801000000</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>20072200</v>
-      </c>
-      <c r="B15" t="n">
-        <v>3601000000</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>20072300</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1199000000</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>20072400</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1734000000</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>20072500</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>20072600</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>20072700</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1750000000</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the first super data is correct
</commit_message>
<xml_diff>
--- a/.idea/fedInvestments.xlsx
+++ b/.idea/fedInvestments.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B364"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,23 +448,23 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>20070900</v>
+        <v>19080100</v>
       </c>
       <c r="B2" t="n">
-        <v>6001000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20071000</v>
+        <v>19080200</v>
       </c>
       <c r="B3" t="n">
-        <v>1201000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>20071100</v>
+        <v>19080300</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -472,7 +472,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>20071200</v>
+        <v>19080400</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>20071300</v>
+        <v>19080500</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -488,39 +488,39 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>20071400</v>
+        <v>19080600</v>
       </c>
       <c r="B7" t="n">
-        <v>1732000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>20071500</v>
+        <v>19080700</v>
       </c>
       <c r="B8" t="n">
-        <v>12801000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>20071600</v>
+        <v>19080800</v>
       </c>
       <c r="B9" t="n">
-        <v>3601000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>20071700</v>
+        <v>19080900</v>
       </c>
       <c r="B10" t="n">
-        <v>1199000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>20071800</v>
+        <v>19081000</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>20071900</v>
+        <v>19081100</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>20072000</v>
+        <v>19081200</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -544,39 +544,39 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>20072100</v>
+        <v>19081300</v>
       </c>
       <c r="B14" t="n">
-        <v>1734000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>20072200</v>
+        <v>19081400</v>
       </c>
       <c r="B15" t="n">
-        <v>6001000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>20072300</v>
+        <v>19081500</v>
       </c>
       <c r="B16" t="n">
-        <v>2401000000</v>
+        <v>3001000000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>20072400</v>
+        <v>19081600</v>
       </c>
       <c r="B17" t="n">
-        <v>1732000000</v>
+        <v>1601000000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>20072500</v>
+        <v>19081700</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>20072600</v>
+        <v>19081800</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -592,47 +592,47 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>20072700</v>
+        <v>19081900</v>
       </c>
       <c r="B20" t="n">
-        <v>8801000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20072800</v>
+        <v>19082000</v>
       </c>
       <c r="B21" t="n">
-        <v>12825000000</v>
+        <v>1801000000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20070100</v>
+        <v>19082100</v>
       </c>
       <c r="B22" t="n">
-        <v>2401000000</v>
+        <v>1801000000</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>20070200</v>
+        <v>19082200</v>
       </c>
       <c r="B23" t="n">
-        <v>3601000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>20070300</v>
+        <v>19082300</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1601000000</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>20070400</v>
+        <v>19082400</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>20070500</v>
+        <v>19082500</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>20070600</v>
+        <v>19082600</v>
       </c>
       <c r="B27" t="n">
         <v>0</v>
@@ -656,23 +656,23 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>20070700</v>
+        <v>19082700</v>
       </c>
       <c r="B28" t="n">
-        <v>12801000000</v>
+        <v>2201000000</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>20070800</v>
+        <v>19082800</v>
       </c>
       <c r="B29" t="n">
-        <v>1732000000</v>
+        <v>2401000000</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>20072900</v>
+        <v>19082900</v>
       </c>
       <c r="B30" t="n">
         <v>0</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>20053000</v>
+        <v>19083000</v>
       </c>
       <c r="B31" t="n">
         <v>0</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>20053100</v>
+        <v>19083100</v>
       </c>
       <c r="B32" t="n">
         <v>0</v>
@@ -696,47 +696,47 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>20060100</v>
+        <v>19090100</v>
       </c>
       <c r="B33" t="n">
-        <v>6500000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>20060200</v>
+        <v>19090200</v>
       </c>
       <c r="B34" t="n">
-        <v>7000000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>20060300</v>
+        <v>19090300</v>
       </c>
       <c r="B35" t="n">
-        <v>3000000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>20060400</v>
+        <v>19090400</v>
       </c>
       <c r="B36" t="n">
-        <v>2100000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>20060500</v>
+        <v>19090500</v>
       </c>
       <c r="B37" t="n">
-        <v>4500000000</v>
+        <v>1401000000</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>20060600</v>
+        <v>19090600</v>
       </c>
       <c r="B38" t="n">
         <v>0</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>20060700</v>
+        <v>19090700</v>
       </c>
       <c r="B39" t="n">
         <v>0</v>
@@ -752,47 +752,47 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>20060800</v>
+        <v>19090800</v>
       </c>
       <c r="B40" t="n">
-        <v>5000000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>20060900</v>
+        <v>19090900</v>
       </c>
       <c r="B41" t="n">
-        <v>2000000000</v>
+        <v>2199000000</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>20061000</v>
+        <v>19091000</v>
       </c>
       <c r="B42" t="n">
-        <v>2750000000</v>
+        <v>1601000000</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>20061100</v>
+        <v>19091100</v>
       </c>
       <c r="B43" t="n">
-        <v>6500000000</v>
+        <v>401000000</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>20061200</v>
+        <v>19091200</v>
       </c>
       <c r="B44" t="n">
-        <v>4000000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>20061300</v>
+        <v>19091300</v>
       </c>
       <c r="B45" t="n">
         <v>0</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>20061400</v>
+        <v>19091400</v>
       </c>
       <c r="B46" t="n">
         <v>0</v>
@@ -808,55 +808,55 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>20061500</v>
+        <v>19091500</v>
       </c>
       <c r="B47" t="n">
-        <v>4401000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>20061600</v>
+        <v>19091600</v>
       </c>
       <c r="B48" t="n">
-        <v>4140000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>20061700</v>
+        <v>19091700</v>
       </c>
       <c r="B49" t="n">
-        <v>25000000</v>
+        <v>1601000000</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>20061800</v>
+        <v>19091800</v>
       </c>
       <c r="B50" t="n">
-        <v>4401000000</v>
+        <v>3001000000</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>20061900</v>
+        <v>19091900</v>
       </c>
       <c r="B51" t="n">
-        <v>3601000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>20062000</v>
+        <v>19092000</v>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>1801000000</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>20062100</v>
+        <v>19092100</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
@@ -864,55 +864,55 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>20062200</v>
+        <v>19092200</v>
       </c>
       <c r="B54" t="n">
-        <v>12801000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>20062300</v>
+        <v>19092300</v>
       </c>
       <c r="B55" t="n">
-        <v>1731000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>20062400</v>
+        <v>19092400</v>
       </c>
       <c r="B56" t="n">
-        <v>6001000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>20062500</v>
+        <v>19092500</v>
       </c>
       <c r="B57" t="n">
-        <v>1201000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>20062600</v>
+        <v>19092600</v>
       </c>
       <c r="B58" t="n">
-        <v>1731000000</v>
+        <v>1801000000</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>20062700</v>
+        <v>19092700</v>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>1601000000</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>20062800</v>
+        <v>19092800</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
@@ -920,18 +920,2434 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>20062900</v>
+        <v>19092900</v>
       </c>
       <c r="B61" t="n">
-        <v>8801000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
+        <v>19093000</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2201000000</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>19100100</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2401000000</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>19100200</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1401000000</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>19100300</v>
+      </c>
+      <c r="B65" t="n">
+        <v>2201000000</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>19100400</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>19100500</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>19100600</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>19100700</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>19100800</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>19100900</v>
+      </c>
+      <c r="B71" t="n">
+        <v>401000000</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>19101000</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>19101100</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>19101200</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>19101300</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>19101400</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>19101500</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>19101600</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>19101700</v>
+      </c>
+      <c r="B79" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>19101800</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1801000000</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>19101900</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>19102000</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>19102100</v>
+      </c>
+      <c r="B83" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>19102200</v>
+      </c>
+      <c r="B84" t="n">
+        <v>1801000000</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>19102300</v>
+      </c>
+      <c r="B85" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>19102400</v>
+      </c>
+      <c r="B86" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>19102500</v>
+      </c>
+      <c r="B87" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>19102600</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>19102700</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>19102800</v>
+      </c>
+      <c r="B90" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>19102900</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2201000000</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>19103000</v>
+      </c>
+      <c r="B92" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>19103100</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>19110100</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2401000000</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>19110200</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>19110300</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>19110400</v>
+      </c>
+      <c r="B97" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>19110500</v>
+      </c>
+      <c r="B98" t="n">
+        <v>1401000000</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>19110600</v>
+      </c>
+      <c r="B99" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>19110700</v>
+      </c>
+      <c r="B100" t="n">
+        <v>2201000000</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>19110800</v>
+      </c>
+      <c r="B101" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>19110900</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>19111000</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>19111100</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>19111200</v>
+      </c>
+      <c r="B105" t="n">
+        <v>3001000000</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>19111300</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>19111400</v>
+      </c>
+      <c r="B107" t="n">
+        <v>401000000</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>19111500</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>19111600</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>19111700</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>19111800</v>
+      </c>
+      <c r="B111" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>19111900</v>
+      </c>
+      <c r="B112" t="n">
+        <v>9102000000</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>19112000</v>
+      </c>
+      <c r="B113" t="n">
+        <v>1801000000</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>19112100</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>19112200</v>
+      </c>
+      <c r="B115" t="n">
+        <v>9302000000</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>19112300</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>19112400</v>
+      </c>
+      <c r="B117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>19112500</v>
+      </c>
+      <c r="B118" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>19112600</v>
+      </c>
+      <c r="B119" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>19112700</v>
+      </c>
+      <c r="B120" t="n">
+        <v>9702000000</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>19112800</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>19112900</v>
+      </c>
+      <c r="B122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>19113000</v>
+      </c>
+      <c r="B123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>19120100</v>
+      </c>
+      <c r="B124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>19120200</v>
+      </c>
+      <c r="B125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>19120300</v>
+      </c>
+      <c r="B126" t="n">
+        <v>2401000000</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>19120400</v>
+      </c>
+      <c r="B127" t="n">
+        <v>8902000000</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>19120500</v>
+      </c>
+      <c r="B128" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>19120600</v>
+      </c>
+      <c r="B129" t="n">
+        <v>2251000000</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>19120700</v>
+      </c>
+      <c r="B130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>19120800</v>
+      </c>
+      <c r="B131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>19120900</v>
+      </c>
+      <c r="B132" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>19121000</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>19121100</v>
+      </c>
+      <c r="B134" t="n">
+        <v>3402000000</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>19121200</v>
+      </c>
+      <c r="B135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>19121300</v>
+      </c>
+      <c r="B136" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>19121400</v>
+      </c>
+      <c r="B137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>19121500</v>
+      </c>
+      <c r="B138" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>19121600</v>
+      </c>
+      <c r="B139" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>19121700</v>
+      </c>
+      <c r="B140" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>19121800</v>
+      </c>
+      <c r="B141" t="n">
+        <v>9302000000</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>19121900</v>
+      </c>
+      <c r="B142" t="n">
+        <v>9302000000</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>19122000</v>
+      </c>
+      <c r="B143" t="n">
+        <v>9102000000</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>19122100</v>
+      </c>
+      <c r="B144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>19122200</v>
+      </c>
+      <c r="B145" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>19122300</v>
+      </c>
+      <c r="B146" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>19122400</v>
+      </c>
+      <c r="B147" t="n">
+        <v>2201000000</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>19122500</v>
+      </c>
+      <c r="B148" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>19122600</v>
+      </c>
+      <c r="B149" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>19122700</v>
+      </c>
+      <c r="B150" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>19122800</v>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>19122900</v>
+      </c>
+      <c r="B152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>19123000</v>
+      </c>
+      <c r="B153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>19123100</v>
+      </c>
+      <c r="B154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>20010100</v>
+      </c>
+      <c r="B155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>20010200</v>
+      </c>
+      <c r="B156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>20010300</v>
+      </c>
+      <c r="B157" t="n">
+        <v>2399000000</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>20010400</v>
+      </c>
+      <c r="B158" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>20010500</v>
+      </c>
+      <c r="B159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>20010600</v>
+      </c>
+      <c r="B160" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>20010700</v>
+      </c>
+      <c r="B161" t="n">
+        <v>1401000000</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>20010800</v>
+      </c>
+      <c r="B162" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>20010900</v>
+      </c>
+      <c r="B163" t="n">
+        <v>7902000000</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>20011000</v>
+      </c>
+      <c r="B164" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>20011100</v>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>20011200</v>
+      </c>
+      <c r="B166" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>20011300</v>
+      </c>
+      <c r="B167" t="n">
+        <v>3001000000</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>20011400</v>
+      </c>
+      <c r="B168" t="n">
+        <v>2199000000</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>20011500</v>
+      </c>
+      <c r="B169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>20011600</v>
+      </c>
+      <c r="B170" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>20011700</v>
+      </c>
+      <c r="B171" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>20011800</v>
+      </c>
+      <c r="B172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>20011900</v>
+      </c>
+      <c r="B173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>20012000</v>
+      </c>
+      <c r="B174" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>20012100</v>
+      </c>
+      <c r="B175" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>20012200</v>
+      </c>
+      <c r="B176" t="n">
+        <v>1801000000</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>20012300</v>
+      </c>
+      <c r="B177" t="n">
+        <v>9302000000</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>20012400</v>
+      </c>
+      <c r="B178" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>20012500</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>20012600</v>
+      </c>
+      <c r="B180" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>20012700</v>
+      </c>
+      <c r="B181" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>20012800</v>
+      </c>
+      <c r="B182" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>20012900</v>
+      </c>
+      <c r="B183" t="n">
+        <v>2201000000</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>20013000</v>
+      </c>
+      <c r="B184" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>20013100</v>
+      </c>
+      <c r="B185" t="n">
+        <v>2399000000</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>20020100</v>
+      </c>
+      <c r="B186" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>20020200</v>
+      </c>
+      <c r="B187" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>20020300</v>
+      </c>
+      <c r="B188" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>20020400</v>
+      </c>
+      <c r="B189" t="n">
+        <v>1401000000</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>20020500</v>
+      </c>
+      <c r="B190" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>20020600</v>
+      </c>
+      <c r="B191" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>20020700</v>
+      </c>
+      <c r="B192" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>20020800</v>
+      </c>
+      <c r="B193" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>20020900</v>
+      </c>
+      <c r="B194" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>20021000</v>
+      </c>
+      <c r="B195" t="n">
+        <v>401000000</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>20021100</v>
+      </c>
+      <c r="B196" t="n">
+        <v>2201000000</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>20021200</v>
+      </c>
+      <c r="B197" t="n">
+        <v>3001000000</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>20021300</v>
+      </c>
+      <c r="B198" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>20021400</v>
+      </c>
+      <c r="B199" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>20021500</v>
+      </c>
+      <c r="B200" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>20021600</v>
+      </c>
+      <c r="B201" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>20021700</v>
+      </c>
+      <c r="B202" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>20021800</v>
+      </c>
+      <c r="B203" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>20021900</v>
+      </c>
+      <c r="B204" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>20022000</v>
+      </c>
+      <c r="B205" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>20022100</v>
+      </c>
+      <c r="B206" t="n">
+        <v>1801000000</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>20022200</v>
+      </c>
+      <c r="B207" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>20022300</v>
+      </c>
+      <c r="B208" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>20022400</v>
+      </c>
+      <c r="B209" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>20022500</v>
+      </c>
+      <c r="B210" t="n">
+        <v>3402000000</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>20022600</v>
+      </c>
+      <c r="B211" t="n">
+        <v>2201000000</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>20022700</v>
+      </c>
+      <c r="B212" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>20022800</v>
+      </c>
+      <c r="B213" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>20022900</v>
+      </c>
+      <c r="B214" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>20030100</v>
+      </c>
+      <c r="B215" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>20030200</v>
+      </c>
+      <c r="B216" t="n">
+        <v>2399000000</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>20030300</v>
+      </c>
+      <c r="B217" t="n">
+        <v>1401000000</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>20030400</v>
+      </c>
+      <c r="B218" t="n">
+        <v>9698000000</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>20030500</v>
+      </c>
+      <c r="B219" t="n">
+        <v>7499000000</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>20030600</v>
+      </c>
+      <c r="B220" t="n">
+        <v>1601000000</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>20030700</v>
+      </c>
+      <c r="B221" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>20030800</v>
+      </c>
+      <c r="B222" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>20030900</v>
+      </c>
+      <c r="B223" t="n">
+        <v>7501000000</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>20031000</v>
+      </c>
+      <c r="B224" t="n">
+        <v>3001000000</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>20031100</v>
+      </c>
+      <c r="B225" t="n">
+        <v>401000000</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>20031200</v>
+      </c>
+      <c r="B226" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>20031300</v>
+      </c>
+      <c r="B227" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>20031400</v>
+      </c>
+      <c r="B228" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>20031500</v>
+      </c>
+      <c r="B229" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>20031600</v>
+      </c>
+      <c r="B230" t="n">
+        <v>37004000000</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>20031700</v>
+      </c>
+      <c r="B231" t="n">
+        <v>40004000000</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>20031800</v>
+      </c>
+      <c r="B232" t="n">
+        <v>40006000000</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>20031900</v>
+      </c>
+      <c r="B233" t="n">
+        <v>45007000000</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>20032000</v>
+      </c>
+      <c r="B234" t="n">
+        <v>74998000000</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>20032100</v>
+      </c>
+      <c r="B235" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>20032200</v>
+      </c>
+      <c r="B236" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>20032300</v>
+      </c>
+      <c r="B237" t="n">
+        <v>72122000000</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>20032400</v>
+      </c>
+      <c r="B238" t="n">
+        <v>73829000000</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>20032500</v>
+      </c>
+      <c r="B239" t="n">
+        <v>68953000000</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>20032600</v>
+      </c>
+      <c r="B240" t="n">
+        <v>70948000000</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>20032700</v>
+      </c>
+      <c r="B241" t="n">
+        <v>73680000000</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>20032800</v>
+      </c>
+      <c r="B242" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>20032900</v>
+      </c>
+      <c r="B243" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>20033000</v>
+      </c>
+      <c r="B244" t="n">
+        <v>71500000000</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>20033100</v>
+      </c>
+      <c r="B245" t="n">
+        <v>71500000000</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>20040100</v>
+      </c>
+      <c r="B246" t="n">
+        <v>72900000000</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>20040200</v>
+      </c>
+      <c r="B247" t="n">
+        <v>72900000000</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>20040300</v>
+      </c>
+      <c r="B248" t="n">
+        <v>58500000000</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>20040400</v>
+      </c>
+      <c r="B249" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>20040500</v>
+      </c>
+      <c r="B250" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>20040600</v>
+      </c>
+      <c r="B251" t="n">
+        <v>58500000000</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>20040700</v>
+      </c>
+      <c r="B252" t="n">
+        <v>46500000000</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>20040800</v>
+      </c>
+      <c r="B253" t="n">
+        <v>55500000000</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>20040900</v>
+      </c>
+      <c r="B254" t="n">
+        <v>52846000000</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>20041000</v>
+      </c>
+      <c r="B255" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>20041100</v>
+      </c>
+      <c r="B256" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>20041200</v>
+      </c>
+      <c r="B257" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>20041300</v>
+      </c>
+      <c r="B258" t="n">
+        <v>38498000000</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>20041400</v>
+      </c>
+      <c r="B259" t="n">
+        <v>29000000000</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>20041500</v>
+      </c>
+      <c r="B260" t="n">
+        <v>33000000000</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>20041600</v>
+      </c>
+      <c r="B261" t="n">
+        <v>31000000000</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>20041700</v>
+      </c>
+      <c r="B262" t="n">
+        <v>27500000000</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>20041800</v>
+      </c>
+      <c r="B263" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>20041900</v>
+      </c>
+      <c r="B264" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>20042000</v>
+      </c>
+      <c r="B265" t="n">
+        <v>29500000000</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>20042100</v>
+      </c>
+      <c r="B266" t="n">
+        <v>15500000000</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>20042200</v>
+      </c>
+      <c r="B267" t="n">
+        <v>16000000000</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>20042300</v>
+      </c>
+      <c r="B268" t="n">
+        <v>7000000000</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>20042400</v>
+      </c>
+      <c r="B269" t="n">
+        <v>20903000000</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>20042500</v>
+      </c>
+      <c r="B270" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>20042600</v>
+      </c>
+      <c r="B271" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>20042700</v>
+      </c>
+      <c r="B272" t="n">
+        <v>15296000000</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>20042800</v>
+      </c>
+      <c r="B273" t="n">
+        <v>6802000000</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>20042900</v>
+      </c>
+      <c r="B274" t="n">
+        <v>11000000000</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>20043000</v>
+      </c>
+      <c r="B275" t="n">
+        <v>7000000000</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>20050100</v>
+      </c>
+      <c r="B276" t="n">
+        <v>14000000000</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>20050200</v>
+      </c>
+      <c r="B277" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>20050300</v>
+      </c>
+      <c r="B278" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>20050400</v>
+      </c>
+      <c r="B279" t="n">
+        <v>10500000000</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>20050500</v>
+      </c>
+      <c r="B280" t="n">
+        <v>3945000000</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>20050600</v>
+      </c>
+      <c r="B281" t="n">
+        <v>13000000000</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>20050700</v>
+      </c>
+      <c r="B282" t="n">
+        <v>6000000000</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>20050800</v>
+      </c>
+      <c r="B283" t="n">
+        <v>8500000000</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>20050900</v>
+      </c>
+      <c r="B284" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>20051000</v>
+      </c>
+      <c r="B285" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>20051100</v>
+      </c>
+      <c r="B286" t="n">
+        <v>8000000000</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>20051200</v>
+      </c>
+      <c r="B287" t="n">
+        <v>3350000000</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>20051300</v>
+      </c>
+      <c r="B288" t="n">
+        <v>11000000000</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>20051400</v>
+      </c>
+      <c r="B289" t="n">
+        <v>5750000000</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>20051500</v>
+      </c>
+      <c r="B290" t="n">
+        <v>6708000000</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>20051600</v>
+      </c>
+      <c r="B291" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>20051700</v>
+      </c>
+      <c r="B292" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>20051800</v>
+      </c>
+      <c r="B293" t="n">
+        <v>7000000000</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>20051900</v>
+      </c>
+      <c r="B294" t="n">
+        <v>2900000000</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>20052000</v>
+      </c>
+      <c r="B295" t="n">
+        <v>9500000000</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>20052100</v>
+      </c>
+      <c r="B296" t="n">
+        <v>5685000000</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>20052200</v>
+      </c>
+      <c r="B297" t="n">
+        <v>4450000000</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>20052300</v>
+      </c>
+      <c r="B298" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>20052400</v>
+      </c>
+      <c r="B299" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>20052500</v>
+      </c>
+      <c r="B300" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>20052600</v>
+      </c>
+      <c r="B301" t="n">
+        <v>6000000000</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>20052700</v>
+      </c>
+      <c r="B302" t="n">
+        <v>4000000000</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>20052800</v>
+      </c>
+      <c r="B303" t="n">
+        <v>3750000000</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>20052900</v>
+      </c>
+      <c r="B304" t="n">
+        <v>4700000000</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>20053000</v>
+      </c>
+      <c r="B305" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>20053100</v>
+      </c>
+      <c r="B306" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>20060100</v>
+      </c>
+      <c r="B307" t="n">
+        <v>6500000000</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>20060200</v>
+      </c>
+      <c r="B308" t="n">
+        <v>7000000000</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>20060300</v>
+      </c>
+      <c r="B309" t="n">
+        <v>3000000000</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>20060400</v>
+      </c>
+      <c r="B310" t="n">
+        <v>2100000000</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>20060500</v>
+      </c>
+      <c r="B311" t="n">
+        <v>4500000000</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>20060600</v>
+      </c>
+      <c r="B312" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>20060700</v>
+      </c>
+      <c r="B313" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>20060800</v>
+      </c>
+      <c r="B314" t="n">
+        <v>5000000000</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>20060900</v>
+      </c>
+      <c r="B315" t="n">
+        <v>2000000000</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>20061000</v>
+      </c>
+      <c r="B316" t="n">
+        <v>2750000000</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>20061100</v>
+      </c>
+      <c r="B317" t="n">
+        <v>6500000000</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>20061200</v>
+      </c>
+      <c r="B318" t="n">
+        <v>4000000000</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>20061300</v>
+      </c>
+      <c r="B319" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>20061400</v>
+      </c>
+      <c r="B320" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>20061500</v>
+      </c>
+      <c r="B321" t="n">
+        <v>4401000000</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>20061600</v>
+      </c>
+      <c r="B322" t="n">
+        <v>4140000000</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>20061700</v>
+      </c>
+      <c r="B323" t="n">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>20061800</v>
+      </c>
+      <c r="B324" t="n">
+        <v>4401000000</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>20061900</v>
+      </c>
+      <c r="B325" t="n">
+        <v>3601000000</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>20062000</v>
+      </c>
+      <c r="B326" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>20062100</v>
+      </c>
+      <c r="B327" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>20062200</v>
+      </c>
+      <c r="B328" t="n">
+        <v>12801000000</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>20062300</v>
+      </c>
+      <c r="B329" t="n">
+        <v>1731000000</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>20062400</v>
+      </c>
+      <c r="B330" t="n">
+        <v>6001000000</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>20062500</v>
+      </c>
+      <c r="B331" t="n">
+        <v>1201000000</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>20062600</v>
+      </c>
+      <c r="B332" t="n">
+        <v>1731000000</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>20062700</v>
+      </c>
+      <c r="B333" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>20062800</v>
+      </c>
+      <c r="B334" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>20062900</v>
+      </c>
+      <c r="B335" t="n">
+        <v>8801000000</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
         <v>20063000</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B336" t="n">
         <v>1735000000</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>20070100</v>
+      </c>
+      <c r="B337" t="n">
+        <v>2401000000</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>20070200</v>
+      </c>
+      <c r="B338" t="n">
+        <v>3601000000</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>20070300</v>
+      </c>
+      <c r="B339" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>20070400</v>
+      </c>
+      <c r="B340" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>20070500</v>
+      </c>
+      <c r="B341" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>20070600</v>
+      </c>
+      <c r="B342" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>20070700</v>
+      </c>
+      <c r="B343" t="n">
+        <v>12801000000</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>20070800</v>
+      </c>
+      <c r="B344" t="n">
+        <v>1732000000</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>20070900</v>
+      </c>
+      <c r="B345" t="n">
+        <v>6001000000</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>20071000</v>
+      </c>
+      <c r="B346" t="n">
+        <v>1201000000</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>20071100</v>
+      </c>
+      <c r="B347" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>20071200</v>
+      </c>
+      <c r="B348" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>20071300</v>
+      </c>
+      <c r="B349" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>20071400</v>
+      </c>
+      <c r="B350" t="n">
+        <v>1732000000</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>20071500</v>
+      </c>
+      <c r="B351" t="n">
+        <v>12801000000</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>20071600</v>
+      </c>
+      <c r="B352" t="n">
+        <v>3601000000</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>20071700</v>
+      </c>
+      <c r="B353" t="n">
+        <v>1199000000</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>20071800</v>
+      </c>
+      <c r="B354" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>20071900</v>
+      </c>
+      <c r="B355" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>20072000</v>
+      </c>
+      <c r="B356" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>20072100</v>
+      </c>
+      <c r="B357" t="n">
+        <v>1734000000</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>20072200</v>
+      </c>
+      <c r="B358" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>20072300</v>
+      </c>
+      <c r="B359" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>20072400</v>
+      </c>
+      <c r="B360" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>20072500</v>
+      </c>
+      <c r="B361" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>20072600</v>
+      </c>
+      <c r="B362" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>20072700</v>
+      </c>
+      <c r="B363" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>20072800</v>
+      </c>
+      <c r="B364" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on the new soma
</commit_message>
<xml_diff>
--- a/.idea/fedInvestments.xlsx
+++ b/.idea/fedInvestments.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B382"/>
+  <dimension ref="A1:B387"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3494,6 +3494,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>20081600</v>
+      </c>
+      <c r="B383" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>20081700</v>
+      </c>
+      <c r="B384" t="n">
+        <v>12801000000</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>20081800</v>
+      </c>
+      <c r="B385" t="n">
+        <v>1732000000</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>20081900</v>
+      </c>
+      <c r="B386" t="n">
+        <v>8825000000</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>20082000</v>
+      </c>
+      <c r="B387" t="n">
+        <v>1225000000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>